<commit_message>
Atualizando a lista de CNPJs
</commit_message>
<xml_diff>
--- a/data/ListaCnpjs.xlsx
+++ b/data/ListaCnpjs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\MyProjects\busca_cnpjs_rf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E8F4DC-99AA-416E-B8D8-6D1A124CCB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886C36D8-2AB5-449F-99C8-450E6F95F8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CNPJs</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>05.208.559/0001-25</t>
-  </si>
-  <si>
-    <t>61.076.055/0001</t>
   </si>
   <si>
     <t>59.981.829/0001-65</t>
@@ -388,11 +385,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -445,11 +440,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>